<commit_message>
chore: update game data via workflow
</commit_message>
<xml_diff>
--- a/projects/LinkedIn_games/LinkedIn_games_data.xlsx
+++ b/projects/LinkedIn_games/LinkedIn_games_data.xlsx
@@ -1,272 +1,265 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hullacuk-my.sharepoint.com/personal/c_ho-2023_hull_ac_uk/Documents/Github/Quarto-Website/PersonalWebsite/projects/LinkedIn_games/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_DEEE713E0089629F144733FA5F7C99CA5C8606D7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5CDACCB-595A-4613-8410-8CF8A8C222D1}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="1095" windowWidth="18000" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="80">
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>CW_T</t>
-  </si>
-  <si>
-    <t>CW_Z</t>
-  </si>
-  <si>
-    <t>CW_P</t>
-  </si>
-  <si>
-    <t>CW_C</t>
-  </si>
-  <si>
-    <t>PM_T</t>
-  </si>
-  <si>
-    <t>PM_Z</t>
-  </si>
-  <si>
-    <t>PM_P</t>
-  </si>
-  <si>
-    <t>PM_C</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>87</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>239</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>260</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>159</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>144</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>219</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>85</t>
-  </si>
-  <si>
-    <t>99</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>167</t>
-  </si>
-  <si>
-    <t>168</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>137</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CW_T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CW_Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CW_P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CW_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM_T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM_Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM_P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">137</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -302,21 +295,12 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -598,16 +582,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:I42"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -636,20 +618,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>45776</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>32</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>105</v>
       </c>
       <c r="F2" t="s">
@@ -665,20 +647,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>45777</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>51</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>47</v>
       </c>
       <c r="F3" t="s">
@@ -694,20 +676,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>45778</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>61</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>37</v>
       </c>
       <c r="F4" t="s">
@@ -723,20 +705,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>45779</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>131</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>46</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>52</v>
       </c>
       <c r="F5" t="s">
@@ -752,20 +734,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>45780</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>154</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="n">
         <v>40</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>82</v>
       </c>
       <c r="F6" t="s">
@@ -781,20 +763,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>45781</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>65</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>85</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>108</v>
       </c>
       <c r="F7" t="s">
@@ -810,20 +792,20 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8">
+      <c r="A8" s="1" t="n">
         <v>45782</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>22</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>41</v>
       </c>
       <c r="F8" t="s">
@@ -839,20 +821,20 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9">
+      <c r="A9" s="1" t="n">
         <v>45783</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>30</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>39</v>
       </c>
       <c r="F9" t="s">
@@ -868,20 +850,20 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10">
+      <c r="A10" s="1" t="n">
         <v>45784</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>37</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>8</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>89</v>
       </c>
       <c r="F10" t="s">
@@ -897,20 +879,20 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11">
+      <c r="A11" s="1" t="n">
         <v>45785</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>40</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>69</v>
       </c>
       <c r="F11" t="s">
@@ -926,20 +908,20 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12">
+      <c r="A12" s="1" t="n">
         <v>45786</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>55</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="n">
         <v>14</v>
       </c>
       <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>36</v>
       </c>
       <c r="F12" t="s">
@@ -955,20 +937,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13">
+      <c r="A13" s="1" t="n">
         <v>45787</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>123</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="n">
         <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>69</v>
       </c>
       <c r="F13" t="s">
@@ -984,20 +966,20 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14">
+      <c r="A14" s="1" t="n">
         <v>45788</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>36</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>49</v>
       </c>
       <c r="D14" t="s">
         <v>26</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>63</v>
       </c>
       <c r="F14" t="s">
@@ -1013,20 +995,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="15">
+      <c r="A15" s="1" t="n">
         <v>45789</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>28</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="n">
         <v>11</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>71</v>
       </c>
       <c r="F15" t="s">
@@ -1042,20 +1024,20 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="16">
+      <c r="A16" s="1" t="n">
         <v>45790</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>31</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="n">
         <v>9</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>49</v>
       </c>
       <c r="F16" t="s">
@@ -1071,20 +1053,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="17">
+      <c r="A17" s="1" t="n">
         <v>45791</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="n">
         <v>64</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="n">
         <v>8</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="n">
         <v>42</v>
       </c>
       <c r="F17" t="s">
@@ -1100,20 +1082,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+    <row r="18">
+      <c r="A18" s="1" t="n">
         <v>45792</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>90</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>246</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="n">
         <v>57</v>
       </c>
       <c r="F18" t="s">
@@ -1129,20 +1111,20 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19">
+      <c r="A19" s="1" t="n">
         <v>45793</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="n">
         <v>30</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="n">
         <v>15</v>
       </c>
       <c r="D19" t="s">
         <v>26</v>
       </c>
-      <c r="E19">
+      <c r="E19" t="n">
         <v>78</v>
       </c>
       <c r="F19" t="s">
@@ -1158,20 +1140,20 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20">
+      <c r="A20" s="1" t="n">
         <v>45794</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="n">
         <v>38</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="n">
         <v>45</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
       </c>
-      <c r="E20">
+      <c r="E20" t="n">
         <v>99</v>
       </c>
       <c r="F20" t="s">
@@ -1187,20 +1169,20 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="21">
+      <c r="A21" s="1" t="n">
         <v>45795</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="n">
         <v>39</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="n">
         <v>54</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
       </c>
-      <c r="E21">
+      <c r="E21" t="n">
         <v>46</v>
       </c>
       <c r="F21" t="s">
@@ -1216,20 +1198,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="22">
+      <c r="A22" s="1" t="n">
         <v>45796</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="n">
         <v>17</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="n">
         <v>22</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22">
+      <c r="E22" t="n">
         <v>64</v>
       </c>
       <c r="F22" t="s">
@@ -1245,20 +1227,20 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="23">
+      <c r="A23" s="1" t="n">
         <v>45797</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="n">
         <v>31</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="n">
         <v>12</v>
       </c>
       <c r="D23" t="s">
         <v>26</v>
       </c>
-      <c r="E23">
+      <c r="E23" t="n">
         <v>38</v>
       </c>
       <c r="F23" t="s">
@@ -1274,20 +1256,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    <row r="24">
+      <c r="A24" s="1" t="n">
         <v>45798</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="n">
         <v>40</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="n">
         <v>17</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
-      <c r="E24">
+      <c r="E24" t="n">
         <v>63</v>
       </c>
       <c r="F24" t="s">
@@ -1303,20 +1285,20 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="25">
+      <c r="A25" s="1" t="n">
         <v>45799</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="n">
         <v>32</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="n">
         <v>46</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="n">
         <v>35</v>
       </c>
       <c r="F25" t="s">
@@ -1332,20 +1314,20 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+    <row r="26">
+      <c r="A26" s="1" t="n">
         <v>45800</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="n">
         <v>60</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="n">
         <v>19</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="n">
         <v>42</v>
       </c>
       <c r="F26" t="s">
@@ -1361,20 +1343,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="27">
+      <c r="A27" s="1" t="n">
         <v>45801</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="n">
         <v>43</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="n">
         <v>27</v>
       </c>
       <c r="D27" t="s">
         <v>26</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="n">
         <v>70</v>
       </c>
       <c r="F27" t="s">
@@ -1390,20 +1372,20 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+    <row r="28">
+      <c r="A28" s="1" t="n">
         <v>45802</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="n">
         <v>40</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="n">
         <v>15</v>
       </c>
       <c r="D28" t="s">
         <v>26</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="n">
         <v>46</v>
       </c>
       <c r="F28" t="s">
@@ -1419,20 +1401,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+    <row r="29">
+      <c r="A29" s="1" t="n">
         <v>45803</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="n">
         <v>19</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="n">
         <v>12</v>
       </c>
       <c r="D29" t="s">
         <v>14</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="n">
         <v>87</v>
       </c>
       <c r="F29" t="s">
@@ -1448,20 +1430,20 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+    <row r="30">
+      <c r="A30" s="1" t="n">
         <v>45804</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="n">
         <v>31</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="n">
         <v>13</v>
       </c>
       <c r="D30" t="s">
         <v>26</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="n">
         <v>46</v>
       </c>
       <c r="F30" t="s">
@@ -1477,20 +1459,20 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="31">
+      <c r="A31" s="1" t="n">
         <v>45805</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="n">
         <v>31</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="n">
         <v>28</v>
       </c>
       <c r="D31" t="s">
         <v>14</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="n">
         <v>45</v>
       </c>
       <c r="F31" t="s">
@@ -1506,20 +1488,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+    <row r="32">
+      <c r="A32" s="1" t="n">
         <v>45806</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="n">
         <v>57</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="n">
         <v>10</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
       </c>
-      <c r="E32">
+      <c r="E32" t="n">
         <v>67</v>
       </c>
       <c r="F32" t="s">
@@ -1535,20 +1517,20 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="33">
+      <c r="A33" s="1" t="n">
         <v>45807</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="n">
         <v>52</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="n">
         <v>11</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
       </c>
-      <c r="E33">
+      <c r="E33" t="n">
         <v>40</v>
       </c>
       <c r="F33" t="s">
@@ -1564,20 +1546,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+    <row r="34">
+      <c r="A34" s="1" t="n">
         <v>45808</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="n">
         <v>117</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="n">
         <v>20</v>
       </c>
       <c r="D34" t="s">
         <v>14</v>
       </c>
-      <c r="E34">
+      <c r="E34" t="n">
         <v>115</v>
       </c>
       <c r="F34" t="s">
@@ -1593,20 +1575,20 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+    <row r="35">
+      <c r="A35" s="1" t="n">
         <v>45809</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="n">
         <v>47</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="n">
         <v>110</v>
       </c>
       <c r="D35" t="s">
         <v>26</v>
       </c>
-      <c r="E35">
+      <c r="E35" t="n">
         <v>60</v>
       </c>
       <c r="F35" t="s">
@@ -1622,20 +1604,20 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="36">
+      <c r="A36" s="1" t="n">
         <v>45810</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="n">
         <v>7</v>
       </c>
-      <c r="C36">
+      <c r="C36" t="n">
         <v>33</v>
       </c>
       <c r="D36" t="s">
         <v>36</v>
       </c>
-      <c r="E36">
+      <c r="E36" t="n">
         <v>31</v>
       </c>
       <c r="F36" t="s">
@@ -1651,20 +1633,20 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+    <row r="37">
+      <c r="A37" s="1" t="n">
         <v>45811</v>
       </c>
-      <c r="B37">
+      <c r="B37" t="n">
         <v>25</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="n">
         <v>10</v>
       </c>
       <c r="D37" t="s">
         <v>36</v>
       </c>
-      <c r="E37">
+      <c r="E37" t="n">
         <v>53</v>
       </c>
       <c r="F37" t="s">
@@ -1680,20 +1662,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+    <row r="38">
+      <c r="A38" s="1" t="n">
         <v>45812</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="n">
         <v>29</v>
       </c>
-      <c r="C38">
+      <c r="C38" t="n">
         <v>10</v>
       </c>
       <c r="D38" t="s">
         <v>26</v>
       </c>
-      <c r="E38">
+      <c r="E38" t="n">
         <v>43</v>
       </c>
       <c r="F38" t="s">
@@ -1709,20 +1691,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+    <row r="39">
+      <c r="A39" s="1" t="n">
         <v>45813</v>
       </c>
-      <c r="B39">
+      <c r="B39" t="n">
         <v>57</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="n">
         <v>8</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
       </c>
-      <c r="E39">
+      <c r="E39" t="n">
         <v>91</v>
       </c>
       <c r="F39" t="s">
@@ -1738,20 +1720,20 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+    <row r="40">
+      <c r="A40" s="1" t="n">
         <v>45814</v>
       </c>
-      <c r="B40">
+      <c r="B40" t="n">
         <v>25</v>
       </c>
-      <c r="C40">
+      <c r="C40" t="n">
         <v>20</v>
       </c>
       <c r="D40" t="s">
         <v>14</v>
       </c>
-      <c r="E40">
+      <c r="E40" t="n">
         <v>88</v>
       </c>
       <c r="F40" t="s">
@@ -1767,14 +1749,38 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>45814</v>
+      </c>
+      <c r="B41" t="n">
+        <v>25</v>
+      </c>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>45814</v>
+      </c>
+      <c r="B42" t="n">
+        <v>25</v>
+      </c>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>